<commit_message>
home code until May 22
</commit_message>
<xml_diff>
--- a/A_results/output.xlsx
+++ b/A_results/output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Seed_42" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,269 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy4/learner_stats/total_loss</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy2/learner_stats/total_loss</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy1/learner_stats/total_loss</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy3/learner_stats/total_loss</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy0/learner_stats/total_loss</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy4/learner_stats/entropy</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy4/learner_stats/entropy_coeff</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy2/learner_stats/entropy</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy2/learner_stats/entropy_coeff</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy1/learner_stats/entropy</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy1/learner_stats/entropy_coeff</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy3/learner_stats/entropy</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy3/learner_stats/entropy_coeff</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy0/learner_stats/entropy</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>info/learner/policy0/learner_stats/entropy_coeff</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>training_iteration</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>episode_len_mean</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>episode_reward_mean</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>9.960103416442871</v>
+      </c>
+      <c r="B2" t="n">
+        <v>9.955968570709228</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9.974653434753415</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9.961173439025879</v>
+      </c>
+      <c r="E2" t="n">
+        <v>9.967659664154052</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.6919238865375519</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.6880520880222321</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.6918735921382904</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.6914673626422883</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.6917753994464875</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>9.959320354461671</v>
+      </c>
+      <c r="B3" t="n">
+        <v>9.9526198387146</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9.750195407867432</v>
+      </c>
+      <c r="D3" t="n">
+        <v>9.939899158477782</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9.860901165008546</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6796949326992034</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.6419391572475434</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.6885584831237793</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.6640703916549683</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.669375067949295</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>80</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-15758.57142857143</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>9.821837902069092</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9.939698123931883</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.779951477050782</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9.944232749938966</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9.973601245880127</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6467763006687164</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.6223031640052795</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.6555776000022888</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.6057752430438995</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.6262050271034241</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>80</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-16992.14285714286</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>